<commit_message>
tumor penetrance stacked grade
</commit_message>
<xml_diff>
--- a/nf1g/surv/pub/tumor_penetrance_stats.xlsx
+++ b/nf1g/surv/pub/tumor_penetrance_stats.xlsx
@@ -411,7 +411,7 @@
         <v>0.05263077017967378</v>
       </c>
       <c r="E2">
-        <v>0.1293987060129399</v>
+        <v>0.1293887061129389</v>
       </c>
       <c r="F2">
         <v>0.1262422127017828</v>
@@ -435,7 +435,7 @@
         <v>0.02531049112083168</v>
       </c>
       <c r="E3">
-        <v>0.005859941400585995</v>
+        <v>0.006509934900650993</v>
       </c>
       <c r="F3">
         <v>0.003496031288069017</v>
@@ -507,7 +507,7 @@
         <v>2.103555533414245E-06</v>
       </c>
       <c r="E6">
-        <v>1.999980000199998E-05</v>
+        <v>9.999900000999991E-06</v>
       </c>
       <c r="F6">
         <v>1.966916540095831E-06</v>
@@ -531,7 +531,7 @@
         <v>4.355878482505148E-05</v>
       </c>
       <c r="E7">
-        <v>9.99990000099999E-05</v>
+        <v>5.999940000599994E-05</v>
       </c>
       <c r="F7">
         <v>1.652519607051981E-05</v>
@@ -627,7 +627,7 @@
         <v>0.1710662537021507</v>
       </c>
       <c r="E11">
-        <v>0.0002399976000239998</v>
+        <v>0.0002099979000209998</v>
       </c>
       <c r="F11">
         <v>0.0003075230499828333</v>
@@ -651,7 +651,7 @@
         <v>0.07079308698188064</v>
       </c>
       <c r="E12">
-        <v>0.1085289147108529</v>
+        <v>0.1082089179108209</v>
       </c>
       <c r="F12">
         <v>0.1301340946313542</v>
@@ -675,7 +675,7 @@
         <v>0.02942546893786807</v>
       </c>
       <c r="E13">
-        <v>0.07439925600743992</v>
+        <v>0.07570924290757093</v>
       </c>
       <c r="F13">
         <v>0.07125765753356648</v>
@@ -723,7 +723,7 @@
         <v>0.5091462715865602</v>
       </c>
       <c r="E15">
-        <v>0.0006999930000699993</v>
+        <v>0.000949990500094999</v>
       </c>
       <c r="F15">
         <v>0.001706611726099423</v>
@@ -747,7 +747,7 @@
         <v>0.6966337870205402</v>
       </c>
       <c r="E16">
-        <v>0.1370386296137039</v>
+        <v>0.1380286197138029</v>
       </c>
       <c r="F16">
         <v>0.1340965212130663</v>
@@ -3756,13 +3756,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ECF54C5-285B-4CA1-BEBB-C981404E900D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36735001-4C81-4052-8FF7-7D38C5CA2343}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6939628C-A8D8-4947-9E29-D104FD76D6C8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27AA03EE-FF99-48A9-A4A6-1300E8A136FA}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60BE2DA7-0F80-455C-9DEC-CE1A742DF425}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0960541A-9DEE-4461-B7E6-76DC578A0F0A}"/>
 </file>
</xml_diff>